<commit_message>
added bloodhound, fixes, plugin name in infos
</commit_message>
<xml_diff>
--- a/pollenisator/Templates/en/Modele.xlsx
+++ b/pollenisator/Templates/en/Modele.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">{{ client }} - {{ contract }}</t>
   </si>
   <si>
-    <t xml:space="preserve">{% for scope in scopes %}{{ scope }}{% endfor %}</t>
+    <t xml:space="preserve">{% for scope in scopes %}{{ scope.scope }}{% endfor %}</t>
   </si>
   <si>
     <t>Identifiant</t>
@@ -46,31 +46,52 @@
     <t>Recommandations</t>
   </si>
   <si>
-    <t xml:space="preserve">Preuves{% for x in defects|selectattr('risk','equalto', 'Critical') %}</t>
+    <t>Preuves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% for x in defects|selectattr('risk','equalto', 'Critical') %}</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
   <si>
     <t xml:space="preserve">D{{  x.id }}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{ x.risk }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ x.ease }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ x.impact }}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{ x.title }}</t>
   </si>
   <si>
-    <t xml:space="preserve">{{ x.ease }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{ x.impact }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{ x.synthesis }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{ x.notes }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{% for instance in x.instances %}{% for para in instance.notes_paragraphs %}{{ para }}{% endfor %}{% endfor %}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{% for instance in x.instances %}{% for proof in instance.proofs %} {{ img proof }}{% endfor %}{% endfor %}</t>
+    <t xml:space="preserve">{{ x.synthesis }}{{ x.notes }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% for instance in x.instances %}{{ instance.notes }}{% else %}{{nothing}}{% endfor %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% for fix in x.fixes %} {{ fix.title }} : {{ fix.synthesis }} {% endfor %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% for instance in x.instances %} {% for proof in instance.proofs %} {% img proof %}{% else %}{{nothing}} {% endfor %} {% endfor %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% endfor %}{% for x in defects|selectattr('risk','equalto', 'Major') %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% for instance in x.instances %} {% for proof in instance.proofs %} {% img proof %} {% else %}{{nothing}}{% endfor %} {% endfor %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% endfor %}{% for x in defects|selectattr('risk','equalto', 'Important') %}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{% endfor %}{% for x in defects|selectattr('risk','equalto', 'Minor') %}</t>
   </si>
   <si>
     <t xml:space="preserve">{% endfor %}</t>
@@ -107,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -148,10 +169,6 @@
     <font>
       <color theme="1"/>
     </font>
-    <font>
-      <name val="Courier New"/>
-      <sz val="10.000000"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -173,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,6 +207,9 @@
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -203,10 +223,28 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -263,8 +301,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Tableau3" ref="A4:I7">
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" displayName="Tableau3" ref="A4:K9">
+  <tableColumns count="11">
     <tableColumn id="1" name="Identifiant" dataDxfId="0"/>
     <tableColumn id="2" name="Risque" dataDxfId="1"/>
     <tableColumn id="3" name="Exploitation" dataDxfId="2"/>
@@ -273,7 +311,9 @@
     <tableColumn id="6" name="Synthèse" dataDxfId="5"/>
     <tableColumn id="7" name="Périmètre" dataDxfId="6"/>
     <tableColumn id="8" name="Recommandations" dataDxfId="7"/>
-    <tableColumn id="9" name="Preuves{% for x in defects|selectattr('risk','equalto', 'Critical') %}" dataDxfId="8"/>
+    <tableColumn id="9" name="Preuves"/>
+    <tableColumn id="10" name="{% for x in defects|selectattr('risk','equalto', 'Critical') %}" dataDxfId="8"/>
+    <tableColumn id="11" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -772,7 +812,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0" zoomScale="100">
+    <sheetView workbookViewId="0" zoomScale="100">
       <selection activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -783,9 +823,9 @@
     <col customWidth="1" min="5" max="5" style="2" width="50.7109375"/>
     <col customWidth="1" min="6" max="6" style="3" width="70.7109375"/>
     <col customWidth="1" min="7" max="7" style="2" width="40.7109375"/>
-    <col customWidth="1" min="8" max="8" style="3" width="50.7109375"/>
-    <col customWidth="1" min="9" max="9" style="2" width="70.7109375"/>
-    <col hidden="1" min="10" max="16384" width="11.42578125"/>
+    <col customWidth="1" min="8" max="9" style="3" width="50.7109375"/>
+    <col customWidth="1" min="10" max="10" style="2" width="70.7109375"/>
+    <col hidden="1" min="11" max="16384" width="11.42578125"/>
   </cols>
   <sheetData>
     <row r="1" ht="24.949999999999999" customHeight="1">
@@ -800,6 +840,7 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" ht="24.949999999999999" customHeight="1">
       <c r="A2" s="5" t="s">
@@ -813,6 +854,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" ht="20.100000000000001" customHeight="1"/>
     <row r="4" ht="20.100000000000001" customHeight="1">
@@ -840,70 +882,196 @@
       <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="J4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" ht="20.100000000000001" hidden="1" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" ht="20.100000000000001" hidden="1" customHeight="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
   </mergeCells>
-  <dataValidations count="5" disablePrompts="0">
-    <dataValidation sqref="C6:C19" type="list" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+  <dataValidations count="11" disablePrompts="0">
+    <dataValidation sqref="C10:C21" type="list" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Valeurs!$A$2:$A$6</formula1>
     </dataValidation>
-    <dataValidation sqref="D6:D19" type="list" allowBlank="1" error="Sélectionner l'impact du défaut de sécurité." errorStyle="stop" errorTitle="Impact invalide" imeMode="noControl" operator="between" prompt="Sélectionner l'impact du défaut de sécurité." promptTitle="Impact" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+    <dataValidation sqref="D10:D21" type="list" allowBlank="1" error="Sélectionner l'impact du défaut de sécurité." errorStyle="stop" errorTitle="Impact invalide" imeMode="noControl" operator="between" prompt="Sélectionner l'impact du défaut de sécurité." promptTitle="Impact" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Valeurs!$B$2:$B$6</formula1>
     </dataValidation>
-    <dataValidation sqref="B6:B18" type="list" allowBlank="1" error="Sélectionner l'impact du défaut de sécurité." errorStyle="stop" errorTitle="Impact invalide" imeMode="noControl" operator="between" prompt="Sélectionner le risque liée à l'exploitation du défaut de sécurité." promptTitle="Risque" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+    <dataValidation sqref="B10:B20" type="list" allowBlank="1" error="Sélectionner l'impact du défaut de sécurité." errorStyle="stop" errorTitle="Impact invalide" imeMode="noControl" operator="between" prompt="Sélectionner le risque liée à l'exploitation du défaut de sécurité." promptTitle="Risque" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Valeurs!$B$2:$B$5</formula1>
     </dataValidation>
     <dataValidation sqref="D5" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Valeurs!$A$2:$A$6</formula1>
     </dataValidation>
     <dataValidation sqref="E5" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Valeurs!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="D8" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Valeurs!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="E8" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Valeurs!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Valeurs!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="E6" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Valeurs!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Valeurs!$A$2:$A$6</formula1>
+    </dataValidation>
+    <dataValidation sqref="E7" type="none" allowBlank="1" error="Sélectionner la facilité d'exploitation du défaut de sécurité." errorStyle="stop" errorTitle="Facilité d'exploitation invalide" imeMode="noControl" operator="between" prompt="Sélectionner la facilité d'exploitation du défaut de sécurité." promptTitle="Facilité d'exploitation" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Valeurs!$A$2:$A$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -918,412 +1086,93 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{00590080-0026-4E19-BEE9-002100610008}">
-            <xm:f>"Critique"</xm:f>
+          <x14:cfRule type="containsText" priority="5" text="Critique" id="{007C0020-005F-46A0-BE25-00550035000B}">
+            <xm:f>NOT(ISERROR(SEARCH("Critique",B4)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="0"/>
+                <b/>
+                <color theme="0" tint="0"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor theme="3"/>
-                  <bgColor theme="3"/>
+                  <fgColor indexed="64"/>
+                  <bgColor indexed="64"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
+          <xm:sqref>B4:D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{000A00F7-00BD-4D19-B7D9-00ED000A0012}">
-            <xm:f>"Critique"</xm:f>
+          <x14:cfRule type="containsText" priority="4" text="Majeur" id="{00F3000C-0056-42F3-A905-00B200B3005D}">
+            <xm:f>NOT(ISERROR(SEARCH("Majeur",B4)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="0"/>
+                <b/>
+                <color theme="0" tint="0"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor theme="3"/>
-                  <bgColor theme="3"/>
+                  <fgColor indexed="2"/>
+                  <bgColor indexed="2"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
+          <xm:sqref>B4:D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="8" operator="equal" id="{00CD005B-00BE-46FA-9BA8-005200FF003C}">
-            <xm:f>"Critique"</xm:f>
+          <x14:cfRule type="containsText" priority="3" text="Important" id="{004500FB-00AC-4002-9329-009700860035}">
+            <xm:f>NOT(ISERROR(SEARCH("Important",B4)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="0"/>
+                <b/>
+                <color theme="0" tint="0"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor theme="3"/>
-                  <bgColor theme="3"/>
+                  <fgColor rgb="FFED7D31"/>
+                  <bgColor rgb="FFED7D31"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B1:D4 B5 D5 B6:D1048576 D5</xm:sqref>
+          <xm:sqref>B4:D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{007F0074-00D1-4E77-899E-009100F200D4}">
-            <xm:f>"Majeur"</xm:f>
+          <x14:cfRule type="containsText" priority="2" text="Mineur" id="{00B900F9-008A-42AE-B100-00B2002E003B}">
+            <xm:f>NOT(ISERROR(SEARCH("Mineur",B4)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="0"/>
+                <b/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFF7453C"/>
-                  <bgColor rgb="FFF7453C"/>
+                  <fgColor rgb="FFFFC000"/>
+                  <bgColor rgb="FFFFC000"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
+          <xm:sqref>B4:D8</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{00CD00A5-002A-4CBB-A77E-00AA00950033}">
-            <xm:f>"Majeur"</xm:f>
+          <x14:cfRule type="containsText" priority="1" text="Facile" id="{000B00DC-00C3-4AAD-AB03-00A2004E00BF}">
+            <xm:f>NOT(ISERROR(SEARCH("Facile",B4)))</xm:f>
             <x14:dxf>
               <font>
-                <color theme="0"/>
+                <b/>
+                <color theme="0" tint="0"/>
               </font>
               <fill>
                 <patternFill patternType="solid">
-                  <fgColor rgb="FFF7453C"/>
-                  <bgColor rgb="FFF7453C"/>
+                  <fgColor indexed="64"/>
+                  <bgColor indexed="64"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>B1:D4 B5 D5 B6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="7" operator="equal" id="{008B0058-0021-4F4F-AAE7-002900920034}">
-            <xm:f>"Majeur"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFF7453C"/>
-                  <bgColor rgb="FFF7453C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{003C00E7-0090-4D68-8C94-003500AA0020}">
-            <xm:f>"Important"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFEE8200"/>
-                  <bgColor rgb="FFEE8200"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>B1:D4 B5 D5 B6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{007C0079-00C0-4C49-A89B-004C00780083}">
-            <xm:f>"Important"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFEE8200"/>
-                  <bgColor rgb="FFEE8200"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="6" operator="equal" id="{008200DF-006D-4A4E-BD36-00C800230056}">
-            <xm:f>"Important"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFEE8200"/>
-                  <bgColor rgb="FFEE8200"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{004900DB-0028-4129-ADE8-00D000080000}">
-            <xm:f>"Mineur"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFD700"/>
-                  <bgColor rgb="FFFFD700"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00230078-004A-4BA0-823E-0063001000D3}">
-            <xm:f>"Mineur"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFD700"/>
-                  <bgColor rgb="FFFFD700"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:D4 A5:B5 D5 A6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{00DA0088-0097-4384-A220-001D00C400C2}">
-            <xm:f>"Mineur"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFD700"/>
-                  <bgColor rgb="FFFFD700"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00BE008B-00CB-40BE-989E-00EC005100BA}">
-            <xm:f>"Facile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF44546A"/>
-                  <bgColor rgb="FF44546A"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00570046-00E9-4284-8DAF-000E005B00D3}">
-            <xm:f>"Facile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF44546A"/>
-                  <bgColor rgb="FF44546A"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:D4 A5:B5 D5 A6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00B700BD-000A-4EF4-B3F2-009200AA00F9}">
-            <xm:f>"Facile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF44546A"/>
-                  <bgColor rgb="FF44546A"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{002C002D-004B-4971-8717-00C300DA00CE}">
-            <xm:f>"Modérée"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFF7453C"/>
-                  <bgColor rgb="FFF7453C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00B80019-00BF-44E4-A345-00340019009C}">
-            <xm:f>"Modérée"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFF7453C"/>
-                  <bgColor rgb="FFF7453C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{000900F6-00FB-4E10-B4C1-00B50027001B}">
-            <xm:f>"Modérée"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFF7453C"/>
-                  <bgColor rgb="FFF7453C"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:D4 A5:B5 D5 A6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00610051-0060-4F93-B626-00A3008800A5}">
-            <xm:f>"Difficile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFEE8200"/>
-                  <bgColor rgb="FFEE8200"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:D4 A5:B5 D5 A6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00FC00D8-00E2-4A5F-9EEF-00B40014003A}">
-            <xm:f>"Difficile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFEE8200"/>
-                  <bgColor rgb="FFEE8200"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00E70098-0070-41CC-9402-0057000C00FB}">
-            <xm:f>"Difficile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFEE8200"/>
-                  <bgColor rgb="FFEE8200"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00EE00B2-007C-4A48-805C-0086004D0098}">
-            <xm:f>"Très difficile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFD700"/>
-                  <bgColor rgb="FFFFD700"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>C5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{00EF00F9-00D9-4EB5-B4F0-008800550004}">
-            <xm:f>"Très difficile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFD700"/>
-                  <bgColor rgb="FFFFD700"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:D4 A5:B5 D5 A6:D1048576 D5</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{008B0048-0073-498F-8C26-009B00AD00ED}">
-            <xm:f>"Très difficile"</xm:f>
-            <x14:dxf>
-              <font>
-                <color theme="1"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFD700"/>
-                  <bgColor rgb="FFFFD700"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E5 E5</xm:sqref>
+          <xm:sqref>B4:D8</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1350,42 +1199,42 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>